<commit_message>
[Ulteriori sviluppi] Raffinati alcuni dettagli 🛠️, preparazione a nuove funzionalità in corso 🚀
</commit_message>
<xml_diff>
--- a/src/example1.xlsx
+++ b/src/example1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="59">
   <si>
     <t>Modulo rilevazione presenza del personale</t>
   </si>
@@ -34,10 +34,10 @@
     <t xml:space="preserve">         Orario Entrata-Uscita</t>
   </si>
   <si>
-    <t xml:space="preserve">      Mattina</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Pomeriggio</t>
+    <t>Mattina</t>
+  </si>
+  <si>
+    <t>Pomeriggio</t>
   </si>
   <si>
     <t>Ore</t>
@@ -65,6 +65,18 @@
   </si>
   <si>
     <t>N O T E</t>
+  </si>
+  <si>
+    <t>GG</t>
+  </si>
+  <si>
+    <t>Ent.</t>
+  </si>
+  <si>
+    <t>Usc.</t>
+  </si>
+  <si>
+    <t>Tot. gg</t>
   </si>
   <si>
     <t>1</t>
@@ -185,7 +197,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -217,6 +229,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <u/>
       <sz val="13"/>
       <color theme="1"/>
@@ -225,6 +244,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="2"/>
@@ -244,12 +270,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="11">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -287,6 +328,17 @@
     </border>
     <border>
       <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color auto="1"/>
       </right>
@@ -294,6 +346,58 @@
         <color auto="1"/>
       </top>
       <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -302,23 +406,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -631,7 +742,7 @@
       <c r="M2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="O2" s="9" t="s">
         <v>2</v>
       </c>
     </row>
@@ -649,417 +760,454 @@
     </row>
     <row r="7" spans="1:15" ht="8" customHeight="1"/>
     <row r="8" spans="1:15">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
       <c r="C8" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="4"/>
     </row>
     <row r="9" spans="1:15">
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="D9" s="6"/>
+      <c r="E9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="F9" s="6"/>
+      <c r="G9" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="J9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="K9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="L9" s="5" t="s">
+      <c r="L9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="M9" s="5" t="s">
+      <c r="M9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="N9" s="5" t="s">
+      <c r="N9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="O9" s="6" t="s">
+      <c r="O9" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:15">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
+      <c r="A10" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="16"/>
     </row>
     <row r="11" spans="1:15">
-      <c r="A11" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="K11" s="8"/>
+      <c r="A11" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="12" spans="1:15">
-      <c r="A12" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>20</v>
+      <c r="A12" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:15">
-      <c r="A13" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="11" t="s">
+      <c r="A13" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="13"/>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="13"/>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
+      <c r="A17" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="A18" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
-      <c r="N13" s="11"/>
-    </row>
-    <row r="14" spans="1:15">
-      <c r="A14" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="11" t="s">
+    </row>
+    <row r="19" spans="1:15">
+      <c r="A19" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11"/>
-      <c r="N14" s="11"/>
-    </row>
-    <row r="15" spans="1:15">
-      <c r="A15" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="10" t="s">
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="12" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="16" spans="1:15">
-      <c r="A16" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="10" t="s">
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="13"/>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="12" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="17" spans="1:14">
-      <c r="A17" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="10" t="s">
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="13"/>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="A22" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
-      <c r="A18" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14">
-      <c r="A19" s="9" t="s">
+    <row r="23" spans="1:15">
+      <c r="A23" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14">
-      <c r="A20" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" s="11" t="s">
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="A25" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="11"/>
-      <c r="L20" s="11"/>
-      <c r="M20" s="11"/>
-      <c r="N20" s="11"/>
-    </row>
-    <row r="21" spans="1:14">
-      <c r="A21" s="9" t="s">
+    </row>
+    <row r="26" spans="1:15">
+      <c r="A26" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
+      <c r="A27" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="13"/>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="A28" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="12"/>
+      <c r="M28" s="12"/>
+      <c r="N28" s="12"/>
+      <c r="O28" s="13"/>
+    </row>
+    <row r="29" spans="1:15">
+      <c r="A29" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
+      <c r="A30" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15">
+      <c r="A31" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="11" t="s">
+    </row>
+    <row r="32" spans="1:15">
+      <c r="A32" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15">
+      <c r="A33" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
-      <c r="M21" s="11"/>
-      <c r="N21" s="11"/>
-    </row>
-    <row r="22" spans="1:14">
-      <c r="A22" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="10" t="s">
+    </row>
+    <row r="34" spans="1:15">
+      <c r="A34" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34" s="12" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="23" spans="1:14">
-      <c r="A23" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B23" s="10" t="s">
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="12"/>
+      <c r="M34" s="12"/>
+      <c r="N34" s="12"/>
+      <c r="O34" s="13"/>
+    </row>
+    <row r="35" spans="1:15">
+      <c r="A35" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35" s="12" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="24" spans="1:14">
-      <c r="A24" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B24" s="10" t="s">
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="12"/>
+      <c r="K35" s="12"/>
+      <c r="L35" s="12"/>
+      <c r="M35" s="12"/>
+      <c r="N35" s="12"/>
+      <c r="O35" s="13"/>
+    </row>
+    <row r="36" spans="1:15">
+      <c r="A36" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B36" s="11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
-      <c r="A25" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14">
-      <c r="A26" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14">
-      <c r="A27" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B27" s="11" t="s">
+    <row r="37" spans="1:15">
+      <c r="A37" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15">
+      <c r="A38" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15">
+      <c r="A39" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B39" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11"/>
-      <c r="K27" s="11"/>
-      <c r="L27" s="11"/>
-      <c r="M27" s="11"/>
-      <c r="N27" s="11"/>
-    </row>
-    <row r="28" spans="1:14">
-      <c r="A28" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B28" s="11" t="s">
+    </row>
+    <row r="40" spans="1:15">
+      <c r="A40" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B40" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
-      <c r="K28" s="11"/>
-      <c r="L28" s="11"/>
-      <c r="M28" s="11"/>
-      <c r="N28" s="11"/>
-    </row>
-    <row r="29" spans="1:14">
-      <c r="A29" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B29" s="10" t="s">
+    </row>
+    <row r="41" spans="1:15">
+      <c r="A41" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B41" s="12" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="30" spans="1:14">
-      <c r="A30" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14">
-      <c r="A31" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14">
-      <c r="A32" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14">
-      <c r="A33" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14">
-      <c r="A34" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B34" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="11"/>
-      <c r="J34" s="11"/>
-      <c r="K34" s="11"/>
-      <c r="L34" s="11"/>
-      <c r="M34" s="11"/>
-      <c r="N34" s="11"/>
-    </row>
-    <row r="35" spans="1:14">
-      <c r="A35" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B35" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11"/>
-      <c r="I35" s="11"/>
-      <c r="J35" s="11"/>
-      <c r="K35" s="11"/>
-      <c r="L35" s="11"/>
-      <c r="M35" s="11"/>
-      <c r="N35" s="11"/>
-    </row>
-    <row r="36" spans="1:14">
-      <c r="A36" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14">
-      <c r="A37" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B37" s="10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14">
-      <c r="A38" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="B38" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14">
-      <c r="A39" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="B39" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14">
-      <c r="A40" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B40" s="10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14">
-      <c r="A41" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="B41" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="11"/>
-      <c r="I41" s="11"/>
-      <c r="J41" s="11"/>
-      <c r="K41" s="11"/>
-      <c r="L41" s="11"/>
-      <c r="M41" s="11"/>
-      <c r="N41" s="11"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="12"/>
+      <c r="H41" s="12"/>
+      <c r="I41" s="12"/>
+      <c r="J41" s="12"/>
+      <c r="K41" s="12"/>
+      <c r="L41" s="12"/>
+      <c r="M41" s="12"/>
+      <c r="N41" s="12"/>
+      <c r="O41" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>